<commit_message>
Added more companies in erpnext companies list excel
</commit_message>
<xml_diff>
--- a/ERPNext companies.xlsx
+++ b/ERPNext companies.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
   <si>
     <t>S.No</t>
   </si>
@@ -76,13 +76,229 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>Business Technology Intelligence Company</t>
+  </si>
+  <si>
+    <t> https://saudi-bti.com/</t>
+  </si>
+  <si>
+    <t> Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Aakvatech Limited </t>
+  </si>
+  <si>
+    <t>http://www.aakvatech.com</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Promantia Business Solutions Pvt. Ltd. </t>
+  </si>
+  <si>
+    <t>http://promantia.in/</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>Tasker Systems Inc.</t>
+  </si>
+  <si>
+    <t>http://www.tasker.ph/</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>New Indictrans Technologies Pvt Ltd</t>
+  </si>
+  <si>
+    <t>Indictranstech</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Software@Work India. Pvt. Ltd </t>
+  </si>
+  <si>
+    <t>https://www.sawindia.com</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Greycube Technologies </t>
+  </si>
+  <si>
+    <t>https://greycube.in</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
+  </si>
+  <si>
+    <t>Indiba Business Solutions </t>
+  </si>
+  <si>
+    <t>www.ibsl-it.com</t>
+  </si>
+  <si>
+    <t>http://8848digital.com/erp-solutions</t>
+  </si>
+  <si>
+    <t>8848 Digital LLP</t>
+  </si>
+  <si>
+    <t>Accurate Systems</t>
+  </si>
+  <si>
+    <t>Home - Accurate Systems</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Again Solutions s.r.o.</t>
+  </si>
+  <si>
+    <t>again.solutions</t>
+  </si>
+  <si>
+    <t>Anther Technologies Pvt Ltd</t>
+  </si>
+  <si>
+    <t>Anther Technologies</t>
+  </si>
+  <si>
+    <t>Buildable LVSYS COPR</t>
+  </si>
+  <si>
+    <t>https://www.buildableworks.com/home</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>Byondwave Consulting Sdn Bhd</t>
+  </si>
+  <si>
+    <t>https://byondwave.com/</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Computerised Accounting Tech</t>
+  </si>
+  <si>
+    <t>https://comatng.com</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Craft Interactive Technology LLC</t>
+  </si>
+  <si>
+    <t>https://craftinteractive.ae/</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Go-Live Solutions</t>
+  </si>
+  <si>
+    <t>https://www.golive-solutions.com/ERPNext</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Modern Transition &amp; Co.</t>
+  </si>
+  <si>
+    <t>https://www.mtc-iq.com</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Momscode Technologies Private Limited</t>
+  </si>
+  <si>
+    <t>momscode.in</t>
+  </si>
+  <si>
+    <t>MultiSolutions</t>
+  </si>
+  <si>
+    <t>https://www.multisolutions.com.sa/</t>
+  </si>
+  <si>
+    <t>Navari Limited</t>
+  </si>
+  <si>
+    <t>https://www.navari.co.ke/</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>nVisionIT</t>
+  </si>
+  <si>
+    <t>nvisionit.mu</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Peniel Technology LLC</t>
+  </si>
+  <si>
+    <t>https://www.penieltech.com/</t>
+  </si>
+  <si>
+    <t>Phamos GmbH</t>
+  </si>
+  <si>
+    <t>phamos.eu</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Sanskar Technolab Private Limited</t>
+  </si>
+  <si>
+    <t>Wahni IT Solutions</t>
+  </si>
+  <si>
+    <t>wahni.com</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Ebkar Technology and Management Solutions</t>
+  </si>
+  <si>
+    <t>https://www.ebkar.ly</t>
+  </si>
+  <si>
+    <t>Libya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +314,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,14 +352,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,74 +750,411 @@
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33">
+        <v>8401265878</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1" display="https://saudi-bti.com/"/>
+    <hyperlink ref="C10" r:id="rId2" display="http://www.aakvatech.com/"/>
+    <hyperlink ref="C13" r:id="rId3" display="https://www.indictranstech.com/"/>
+    <hyperlink ref="C14" r:id="rId4" display="https://www.sawindia.com/"/>
+    <hyperlink ref="C15" r:id="rId5" display="https://greycube.in/"/>
+    <hyperlink ref="C16" r:id="rId6" display="https://erpnext.com/partners/india/www.ibsl-it.com"/>
+    <hyperlink ref="C17" r:id="rId7"/>
+    <hyperlink ref="C18" r:id="rId8" display="https://accuratesystems.com.sa/"/>
+    <hyperlink ref="C20" r:id="rId9" display="https://www.anther.tech/"/>
+    <hyperlink ref="C21" r:id="rId10"/>
+    <hyperlink ref="C22" r:id="rId11"/>
+    <hyperlink ref="C23" r:id="rId12" display="https://comatng.com/"/>
+    <hyperlink ref="C24" r:id="rId13"/>
+    <hyperlink ref="C25" r:id="rId14"/>
+    <hyperlink ref="C26" r:id="rId15" display="https://www.mtc-iq.com/"/>
+    <hyperlink ref="C28" r:id="rId16"/>
+    <hyperlink ref="C29" r:id="rId17"/>
+    <hyperlink ref="C31" r:id="rId18"/>
+    <hyperlink ref="C35" r:id="rId19" display="https://www.ebkar.ly/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>